<commit_message>
LED SWITCH ANALOG PWM DIGITAL OUT TEST OK
</commit_message>
<xml_diff>
--- a/Doc/Tim.xlsx
+++ b/Doc/Tim.xlsx
@@ -3,23 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditya\STM32CubeIDE\workspace_1.8.0\LINK4_G070R_TEST_BOARD1\Doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA1EE14-D3E0-44B0-837D-F808C0BC599F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{AB551DCD-0E30-473C-8A6B-E6A49F8EBE70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{3BBC16BF-3852-4B14-B8FB-5FFEF6517710}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20790" windowHeight="11820" tabRatio="779" xr2:uid="{3BBC16BF-3852-4B14-B8FB-5FFEF6517710}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fram" sheetId="4" r:id="rId1"/>
+    <sheet name="Basic Test" sheetId="4" r:id="rId1"/>
     <sheet name="key" sheetId="3" r:id="rId2"/>
     <sheet name="Light" sheetId="1" r:id="rId3"/>
     <sheet name="Remote Tim" sheetId="2" r:id="rId4"/>
     <sheet name="remote hex" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <oleSize ref="B1:R14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>1 us  calcute</t>
   </si>
@@ -97,33 +93,6 @@
     <t>light2 dec</t>
   </si>
   <si>
-    <t>uint32_t mLight1Perc;</t>
-  </si>
-  <si>
-    <t>uint32_t mLight2Perc;</t>
-  </si>
-  <si>
-    <t>uint32_t mMin;</t>
-  </si>
-  <si>
-    <t>uint32_t mMax;</t>
-  </si>
-  <si>
-    <t>uint32_t mStep;</t>
-  </si>
-  <si>
-    <t>uint32_t mIsOn;</t>
-  </si>
-  <si>
-    <t>uint32_t mMode;</t>
-  </si>
-  <si>
-    <t>uint32_t mCurUser;</t>
-  </si>
-  <si>
-    <t>TOTAL FRAM REQ</t>
-  </si>
-  <si>
     <t>37</t>
   </si>
   <si>
@@ -172,9 +141,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>USER DATA CNT</t>
-  </si>
-  <si>
     <t>t up</t>
   </si>
   <si>
@@ -215,6 +181,27 @@
   </si>
   <si>
     <t>mcu pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED </t>
+  </si>
+  <si>
+    <t>SWITCH</t>
+  </si>
+  <si>
+    <t>DIGITAL OUT</t>
+  </si>
+  <si>
+    <t>ANALOG 0-4</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>BASIC UART TEST</t>
+  </si>
+  <si>
+    <t>MODBUS</t>
   </si>
 </sst>
 </file>
@@ -379,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -424,9 +411,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -783,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15B23F8-B338-4788-8888-34FC64A43006}">
-  <dimension ref="E5:T30"/>
+  <dimension ref="E3:T30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,299 +783,133 @@
     <col min="14" max="14" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E5" s="18">
+    <row r="3" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="17">
         <v>1</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="17">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="17">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="17">
         <v>4</v>
       </c>
-      <c r="J5" s="18">
-        <v>11</v>
-      </c>
-      <c r="K5" s="18">
-        <f>(G5+J5)-1</f>
-        <v>14</v>
-      </c>
-      <c r="M5" s="18">
-        <v>4</v>
-      </c>
-      <c r="O5" s="18">
-        <v>11</v>
-      </c>
-      <c r="P5" s="18">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="18">
-        <v>13</v>
-      </c>
-      <c r="R5" s="18">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E6" s="18">
-        <v>2</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="10">
-        <v>4</v>
-      </c>
-      <c r="J6" s="18">
-        <f>K5+1</f>
-        <v>15</v>
-      </c>
-      <c r="K6" s="18">
-        <f t="shared" ref="K6:K9" si="0">(G6+J6)-1</f>
-        <v>18</v>
-      </c>
-      <c r="M6" s="18">
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="17">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="17">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="17">
         <v>8</v>
       </c>
-      <c r="O6" s="18">
-        <v>15</v>
-      </c>
-      <c r="P6" s="18">
-        <v>16</v>
-      </c>
-      <c r="Q6" s="18">
-        <v>17</v>
-      </c>
-      <c r="R6" s="18">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E7" s="18">
-        <v>3</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="10">
-        <v>4</v>
-      </c>
-      <c r="J7" s="18">
-        <f t="shared" ref="J7:J9" si="1">K6+1</f>
-        <v>19</v>
-      </c>
-      <c r="K7" s="18">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="M7" s="18">
-        <v>12</v>
-      </c>
-      <c r="O7" s="18">
-        <v>19</v>
-      </c>
-      <c r="P7" s="18">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="18">
-        <v>21</v>
-      </c>
-      <c r="R7" s="18">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E8" s="18">
-        <v>4</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="10">
-        <v>4</v>
-      </c>
-      <c r="J8" s="18">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="K8" s="18">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="M8" s="18">
-        <v>16</v>
-      </c>
-      <c r="O8" s="18">
-        <v>23</v>
-      </c>
-      <c r="P8" s="18">
-        <v>24</v>
-      </c>
-      <c r="Q8" s="18">
-        <v>25</v>
-      </c>
-      <c r="R8" s="18">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E9" s="18">
-        <v>5</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="10">
-        <v>4</v>
-      </c>
-      <c r="J9" s="18">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="K9" s="18">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="M9" s="18">
-        <v>20</v>
-      </c>
-      <c r="O9" s="18">
-        <v>27</v>
-      </c>
-      <c r="P9" s="18">
-        <v>28</v>
-      </c>
-      <c r="Q9" s="18">
-        <v>29</v>
-      </c>
-      <c r="R9" s="18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E10" s="18"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="14">
-        <f>SUM(G5:G9)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="G13">
-        <f>G10*G12</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E15" s="18">
-        <v>1</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E16" s="18">
-        <v>2</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E17" s="18">
-        <v>3</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E18" s="18"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E19" s="18"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="14">
-        <f>SUM(G15:G17)</f>
-        <v>12</v>
-      </c>
-      <c r="Q19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="Q20">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="21" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="Q21">
-        <f>Q19*Q20</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="22" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22">
-        <f>G19+G13</f>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="T23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="T25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="T26">
-        <f>T25*365</f>
-        <v>730</v>
-      </c>
-    </row>
-    <row r="27" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="T27">
-        <f>T26*24</f>
-        <v>17520</v>
-      </c>
-    </row>
-    <row r="28" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="T28">
-        <f>T27*60</f>
-        <v>1051200</v>
-      </c>
-    </row>
-    <row r="30" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="T30">
-        <f>T28/10</f>
-        <v>105120</v>
-      </c>
+    </row>
+    <row r="12" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="17"/>
+    </row>
+    <row r="16" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="17"/>
+    </row>
+    <row r="21" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="17"/>
+    </row>
+    <row r="30" spans="5:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1167,11 +985,11 @@
     <row r="14" spans="5:20" x14ac:dyDescent="0.25">
       <c r="K14" s="10"/>
       <c r="L14" s="10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="O14" s="10"/>
     </row>
@@ -1194,11 +1012,11 @@
     <row r="16" spans="5:20" x14ac:dyDescent="0.25">
       <c r="K16" s="10"/>
       <c r="L16" s="10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="10" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="O16" s="10"/>
       <c r="R16">
@@ -1215,11 +1033,11 @@
     <row r="17" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K17" s="10"/>
       <c r="L17" s="10" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="10" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="O17" s="10"/>
       <c r="R17">
@@ -1229,11 +1047,11 @@
     <row r="18" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K18" s="10"/>
       <c r="L18" s="10" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="10" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="O18" s="10"/>
       <c r="R18">
@@ -1249,11 +1067,11 @@
     <row r="19" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K19" s="10"/>
       <c r="L19" s="10" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="O19" s="10"/>
       <c r="R19">
@@ -1272,22 +1090,22 @@
     <row r="20" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K20" s="10"/>
       <c r="L20" s="10" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="10" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="O20" s="10"/>
     </row>
     <row r="21" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K21" s="10"/>
       <c r="L21" s="10" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="10" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="O21" s="10"/>
       <c r="S21">
@@ -1330,7 +1148,7 @@
   <dimension ref="D4:H985"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,7 +1157,7 @@
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="10" width="8.7109375" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" customWidth="1"/>
@@ -1370,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="15">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="10"/>
@@ -1380,7 +1198,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="1">
         <f>E6*1000000</f>
-        <v>48000000</v>
+        <v>64000000</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="10"/>
@@ -1391,7 +1209,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="16">
-        <v>1600</v>
+        <v>64</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="10"/>
@@ -1410,7 +1228,7 @@
       </c>
       <c r="E10" s="1">
         <f>E7/E8</f>
-        <v>30000</v>
+        <v>1000000</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="10"/>
@@ -1432,7 +1250,7 @@
       </c>
       <c r="F12" s="9">
         <f>(E12+1)/E10</f>
-        <v>6.666666666666667E-5</v>
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1442,15 +1260,16 @@
         <v>5</v>
       </c>
       <c r="E13" s="1">
-        <v>200</v>
+        <f>999+1</f>
+        <v>1000</v>
       </c>
       <c r="F13" s="9">
         <f>(E13+1)/E10</f>
-        <v>6.7000000000000002E-3</v>
+        <v>1.0009999999999999E-3</v>
       </c>
       <c r="G13" s="13">
         <f>E10/E13</f>
-        <v>150</v>
+        <v>1000</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>10</v>
@@ -1465,7 +1284,7 @@
       </c>
       <c r="F14" s="9">
         <f>(E14+1)/E10</f>
-        <v>3.6666666666666667E-4</v>
+        <v>1.1E-5</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -1479,7 +1298,7 @@
       </c>
       <c r="F15" s="9">
         <f>(E15+1)/E10</f>
-        <v>6.3666666666666663E-3</v>
+        <v>1.9100000000000001E-4</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -2464,8 +2283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B9321E-0F89-4257-8D80-A27D23B097B6}">
   <dimension ref="D3:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,22 +2296,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
@@ -2663,48 +2482,48 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="A4" s="18">
         <v>1</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="21" t="str">
+      <c r="B4" s="18"/>
+      <c r="C4" s="20" t="str">
         <f>_xlfn.CONCAT("0x",C3)</f>
         <v>0x37</v>
       </c>
-      <c r="D4" s="21" t="str">
+      <c r="D4" s="20" t="str">
         <f>_xlfn.CONCAT("0x",D3)</f>
         <v>0x44</v>
       </c>
-      <c r="E4" s="21" t="str">
+      <c r="E4" s="20" t="str">
         <f>_xlfn.CONCAT("0x",E3)</f>
         <v>0x38</v>
       </c>
-      <c r="F4" s="21" t="str">
+      <c r="F4" s="20" t="str">
         <f>_xlfn.CONCAT("0x",F3)</f>
         <v>0x32</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19" t="str">
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C4,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D4,0)," &amp;&amp; ",
@@ -2714,59 +2533,59 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>2</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="21" t="str">
+      <c r="B7" s="18"/>
+      <c r="C7" s="20" t="str">
         <f>_xlfn.CONCAT("0x",C6)</f>
         <v>0x37</v>
       </c>
-      <c r="D7" s="21" t="str">
+      <c r="D7" s="20" t="str">
         <f>_xlfn.CONCAT("0x",D6)</f>
         <v>0x35</v>
       </c>
-      <c r="E7" s="21" t="str">
+      <c r="E7" s="20" t="str">
         <f>_xlfn.CONCAT("0x",E6)</f>
         <v>0x38</v>
       </c>
-      <c r="F7" s="21" t="str">
+      <c r="F7" s="20" t="str">
         <f>_xlfn.CONCAT("0x",F6)</f>
         <v>0x41</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19" t="str">
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C7,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D7,0)," &amp;&amp; ",
@@ -2776,59 +2595,59 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="18">
         <v>3</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="21" t="str">
+      <c r="B10" s="18"/>
+      <c r="C10" s="20" t="str">
         <f>_xlfn.CONCAT("0x",C9)</f>
         <v>0x37</v>
       </c>
-      <c r="D10" s="21" t="str">
+      <c r="D10" s="20" t="str">
         <f>_xlfn.CONCAT("0x",D9)</f>
         <v>0x39</v>
       </c>
-      <c r="E10" s="21" t="str">
+      <c r="E10" s="20" t="str">
         <f>_xlfn.CONCAT("0x",E9)</f>
         <v>0x38</v>
       </c>
-      <c r="F10" s="21" t="str">
+      <c r="F10" s="20" t="str">
         <f>_xlfn.CONCAT("0x",F9)</f>
         <v>0x36</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19" t="str">
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C10,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D10,0)," &amp;&amp; ",
@@ -2838,48 +2657,48 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="24" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
+      <c r="F12" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
+      <c r="A13" s="22">
         <v>4</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="25" t="str">
+      <c r="B13" s="22"/>
+      <c r="C13" s="24" t="str">
         <f>_xlfn.CONCAT("0x",C12)</f>
         <v>0x46</v>
       </c>
-      <c r="D13" s="25" t="str">
+      <c r="D13" s="24" t="str">
         <f>_xlfn.CONCAT("0x",D12)</f>
         <v>0x38</v>
       </c>
-      <c r="E13" s="25" t="str">
+      <c r="E13" s="24" t="str">
         <f>_xlfn.CONCAT("0x",E12)</f>
         <v>0x30</v>
       </c>
-      <c r="F13" s="25" t="str">
+      <c r="F13" s="24" t="str">
         <f>_xlfn.CONCAT("0x",F12)</f>
         <v>0x37</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23" t="str">
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C13,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D13,0)," &amp;&amp; ",
@@ -2889,59 +2708,59 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
+      <c r="A16" s="22">
         <v>5</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="25" t="str">
+      <c r="B16" s="22"/>
+      <c r="C16" s="24" t="str">
         <f>_xlfn.CONCAT("0x",C15)</f>
         <v>0x46</v>
       </c>
-      <c r="D16" s="25" t="str">
+      <c r="D16" s="24" t="str">
         <f>_xlfn.CONCAT("0x",D15)</f>
         <v>0x34</v>
       </c>
-      <c r="E16" s="25" t="str">
+      <c r="E16" s="24" t="str">
         <f>_xlfn.CONCAT("0x",E15)</f>
         <v>0x30</v>
       </c>
-      <c r="F16" s="25" t="str">
+      <c r="F16" s="24" t="str">
         <f>_xlfn.CONCAT("0x",F15)</f>
         <v>0x42</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23" t="str">
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C16,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D16,0)," &amp;&amp; ",
@@ -2951,59 +2770,59 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="23">
+      <c r="A19" s="22">
         <v>6</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="25" t="str">
+      <c r="B19" s="22"/>
+      <c r="C19" s="24" t="str">
         <f>_xlfn.CONCAT("0x",C18)</f>
         <v>0x46</v>
       </c>
-      <c r="D19" s="25" t="str">
+      <c r="D19" s="24" t="str">
         <f>_xlfn.CONCAT("0x",D18)</f>
         <v>0x43</v>
       </c>
-      <c r="E19" s="25" t="str">
+      <c r="E19" s="24" t="str">
         <f>_xlfn.CONCAT("0x",E18)</f>
         <v>0x30</v>
       </c>
-      <c r="F19" s="25" t="str">
+      <c r="F19" s="24" t="str">
         <f>_xlfn.CONCAT("0x",F18)</f>
         <v>0x33</v>
       </c>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23" t="str">
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C19,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D19,0)," &amp;&amp; ",
@@ -3013,48 +2832,48 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
+      <c r="A22" s="26">
         <v>7</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="29" t="str">
+      <c r="B22" s="26"/>
+      <c r="C22" s="28" t="str">
         <f>_xlfn.CONCAT("0x",C21)</f>
         <v>0x46</v>
       </c>
-      <c r="D22" s="29" t="str">
+      <c r="D22" s="28" t="str">
         <f>_xlfn.CONCAT("0x",D21)</f>
         <v>0x41</v>
       </c>
-      <c r="E22" s="29" t="str">
+      <c r="E22" s="28" t="str">
         <f>_xlfn.CONCAT("0x",E21)</f>
         <v>0x30</v>
       </c>
-      <c r="F22" s="29" t="str">
+      <c r="F22" s="28" t="str">
         <f>_xlfn.CONCAT("0x",F21)</f>
         <v>0x35</v>
       </c>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27" t="str">
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C22,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D22,0)," &amp;&amp; ",
@@ -3064,59 +2883,59 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="27">
+      <c r="A25" s="26">
         <v>8</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="29" t="str">
+      <c r="B25" s="26"/>
+      <c r="C25" s="28" t="str">
         <f>_xlfn.CONCAT("0x",C24)</f>
         <v>0x46</v>
       </c>
-      <c r="D25" s="29" t="str">
+      <c r="D25" s="28" t="str">
         <f>_xlfn.CONCAT("0x",D24)</f>
         <v>0x36</v>
       </c>
-      <c r="E25" s="29" t="str">
+      <c r="E25" s="28" t="str">
         <f>_xlfn.CONCAT("0x",E24)</f>
         <v>0x30</v>
       </c>
-      <c r="F25" s="29" t="str">
+      <c r="F25" s="28" t="str">
         <f>_xlfn.CONCAT("0x",F24)</f>
         <v>0x39</v>
       </c>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27" t="str">
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C25,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D25,0)," &amp;&amp; ",
@@ -3126,59 +2945,59 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="27">
+      <c r="A28" s="26">
         <v>9</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="29" t="str">
+      <c r="B28" s="26"/>
+      <c r="C28" s="28" t="str">
         <f>_xlfn.CONCAT("0x",C27)</f>
         <v>0x46</v>
       </c>
-      <c r="D28" s="29" t="str">
+      <c r="D28" s="28" t="str">
         <f>_xlfn.CONCAT("0x",D27)</f>
         <v>0x45</v>
       </c>
-      <c r="E28" s="29" t="str">
+      <c r="E28" s="28" t="str">
         <f>_xlfn.CONCAT("0x",E27)</f>
         <v>0x30</v>
       </c>
-      <c r="F28" s="29" t="str">
+      <c r="F28" s="28" t="str">
         <f>_xlfn.CONCAT("0x",F27)</f>
         <v>0x31</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27" t="str">
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C28,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D28,0)," &amp;&amp; ",
@@ -3188,48 +3007,48 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
+      <c r="A31" s="18">
         <v>10</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="21" t="str">
+      <c r="B31" s="18"/>
+      <c r="C31" s="20" t="str">
         <f>_xlfn.CONCAT("0x",C30)</f>
         <v>0x46</v>
       </c>
-      <c r="D31" s="21" t="str">
+      <c r="D31" s="20" t="str">
         <f>_xlfn.CONCAT("0x",D30)</f>
         <v>0x39</v>
       </c>
-      <c r="E31" s="21" t="str">
+      <c r="E31" s="20" t="str">
         <f>_xlfn.CONCAT("0x",E30)</f>
         <v>0x30</v>
       </c>
-      <c r="F31" s="21" t="str">
+      <c r="F31" s="20" t="str">
         <f>_xlfn.CONCAT("0x",F30)</f>
         <v>0x36</v>
       </c>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19" t="str">
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C31,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D31,0)," &amp;&amp; ",
@@ -3239,59 +3058,59 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="19">
+      <c r="A34" s="18">
         <v>11</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="21" t="str">
+      <c r="B34" s="18"/>
+      <c r="C34" s="20" t="str">
         <f>_xlfn.CONCAT("0x",C33)</f>
         <v>0x46</v>
       </c>
-      <c r="D34" s="21" t="str">
+      <c r="D34" s="20" t="str">
         <f>_xlfn.CONCAT("0x",D33)</f>
         <v>0x35</v>
       </c>
-      <c r="E34" s="21" t="str">
+      <c r="E34" s="20" t="str">
         <f>_xlfn.CONCAT("0x",E33)</f>
         <v>0x30</v>
       </c>
-      <c r="F34" s="21" t="str">
+      <c r="F34" s="20" t="str">
         <f>_xlfn.CONCAT("0x",F33)</f>
         <v>0x41</v>
       </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19" t="str">
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C34,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D34,0)," &amp;&amp; ",
@@ -3301,59 +3120,59 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="19">
+      <c r="A37" s="18">
         <v>12</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="21" t="str">
+      <c r="B37" s="18"/>
+      <c r="C37" s="20" t="str">
         <f>_xlfn.CONCAT("0x",C36)</f>
         <v>0x46</v>
       </c>
-      <c r="D37" s="21" t="str">
+      <c r="D37" s="20" t="str">
         <f>_xlfn.CONCAT("0x",D36)</f>
         <v>0x44</v>
       </c>
-      <c r="E37" s="21" t="str">
+      <c r="E37" s="20" t="str">
         <f>_xlfn.CONCAT("0x",E36)</f>
         <v>0x30</v>
       </c>
-      <c r="F37" s="21" t="str">
+      <c r="F37" s="20" t="str">
         <f>_xlfn.CONCAT("0x",F36)</f>
         <v>0x32</v>
       </c>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19" t="str">
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18" t="str">
         <f>_xlfn.CONCAT("(",
 "gDecToHex[0]==",TEXT(C37,0)," &amp;&amp; ",
 "gDecToHex[1]==",TEXT(D37,0)," &amp;&amp; ",

</xml_diff>